<commit_message>
Change tab names to survey code in test data xlsx
</commit_message>
<xml_diff>
--- a/packages/meditrak-server/src/tests/testData/surveyResponses/functionality/periodicBaseline.xlsx
+++ b/packages/meditrak-server/src/tests/testData/surveyResponses/functionality/periodicBaseline.xlsx
@@ -1,23 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25003"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kostas/bes/Tupaia/tupaia/packages/meditrak-server/src/tests/testData/surveyResponses/functionality/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118B1ABC-4AD0-E543-8DFC-44A8EF829866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC2BD57C-47AD-4CFC-871D-935E27971988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18960" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18960" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Yearly" sheetId="1" r:id="rId1"/>
-    <sheet name="Test Weekly" sheetId="2" r:id="rId2"/>
+    <sheet name="Test_Yearly" sheetId="1" r:id="rId1"/>
+    <sheet name="Test_Weekly" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -216,18 +226,78 @@
     <t>2017_dl1_dog_delete</t>
   </si>
   <si>
+    <t>2020W2_dl1_untouch__test</t>
+  </si>
+  <si>
+    <t>2020W2_dl1_update___test</t>
+  </si>
+  <si>
+    <t>2020W3_dl1_merge____test</t>
+  </si>
+  <si>
+    <t>2020W2_dl5_override_test</t>
+  </si>
+  <si>
+    <t>2020W2_dl5_merge____test</t>
+  </si>
+  <si>
+    <t>2020W3_dl5_update___test</t>
+  </si>
+  <si>
+    <t>2017W1_dl1_delete___test</t>
+  </si>
+  <si>
     <t>6-1-2020 2:00pm</t>
   </si>
   <si>
+    <t>10-1-2020 2:00pm</t>
+  </si>
+  <si>
+    <t>13-1-2020 2:00pm</t>
+  </si>
+  <si>
+    <t>7-1-2020 2:00pm</t>
+  </si>
+  <si>
+    <t>2-1-2017 2:00pm</t>
+  </si>
+  <si>
+    <t>weekly_bird_________test</t>
+  </si>
+  <si>
+    <t>Test_Weekly_Bird</t>
+  </si>
+  <si>
+    <t>Weekly Bird population</t>
+  </si>
+  <si>
     <t>2020W2_dl1_bird_untouched</t>
   </si>
   <si>
+    <t>2020W3_dl1_bird_existing</t>
+  </si>
+  <si>
+    <t>2020W2_dl5_bird_override_old</t>
+  </si>
+  <si>
+    <t>2020W3_dl5_bird_existing</t>
+  </si>
+  <si>
+    <t>2017W1_dl1_bird_delete</t>
+  </si>
+  <si>
+    <t>weekly_cat__________test</t>
+  </si>
+  <si>
+    <t>Test_Weekly_Cat</t>
+  </si>
+  <si>
+    <t>Weekly Cat population</t>
+  </si>
+  <si>
     <t>2020W2_dl1_cat_untouched</t>
   </si>
   <si>
-    <t>2020W2_dl5_bird_override_old</t>
-  </si>
-  <si>
     <t>2020W2_dl1_cat_existing</t>
   </si>
   <si>
@@ -237,89 +307,29 @@
     <t>2020W2_dl5_cat_existing</t>
   </si>
   <si>
-    <t>2020W3_dl1_bird_existing</t>
-  </si>
-  <si>
-    <t>2020W3_dl5_bird_existing</t>
+    <t>2017W1_dl1_cat_delete</t>
+  </si>
+  <si>
+    <t>weekly_dog__________test</t>
+  </si>
+  <si>
+    <t>Test_Weekly_Dog</t>
+  </si>
+  <si>
+    <t>Weekly Dog population</t>
   </si>
   <si>
     <t>2020W3_dl1_dog_existing</t>
   </si>
   <si>
-    <t>2-1-2017 2:00pm</t>
-  </si>
-  <si>
-    <t>2017W1_dl1_bird_delete</t>
-  </si>
-  <si>
-    <t>2017W1_dl1_cat_delete</t>
-  </si>
-  <si>
     <t>2017W1_dl1_dog_delete</t>
-  </si>
-  <si>
-    <t>13-1-2020 2:00pm</t>
-  </si>
-  <si>
-    <t>10-1-2020 2:00pm</t>
-  </si>
-  <si>
-    <t>7-1-2020 2:00pm</t>
-  </si>
-  <si>
-    <t>2020W2_dl1_untouch__test</t>
-  </si>
-  <si>
-    <t>2020W2_dl1_update___test</t>
-  </si>
-  <si>
-    <t>2020W3_dl1_merge____test</t>
-  </si>
-  <si>
-    <t>2020W2_dl5_override_test</t>
-  </si>
-  <si>
-    <t>2020W2_dl5_merge____test</t>
-  </si>
-  <si>
-    <t>2020W3_dl5_update___test</t>
-  </si>
-  <si>
-    <t>2017W1_dl1_delete___test</t>
-  </si>
-  <si>
-    <t>Test_Weekly_Bird</t>
-  </si>
-  <si>
-    <t>Weekly Bird population</t>
-  </si>
-  <si>
-    <t>Test_Weekly_Cat</t>
-  </si>
-  <si>
-    <t>Weekly Cat population</t>
-  </si>
-  <si>
-    <t>Test_Weekly_Dog</t>
-  </si>
-  <si>
-    <t>Weekly Dog population</t>
-  </si>
-  <si>
-    <t>weekly_bird_________test</t>
-  </si>
-  <si>
-    <t>weekly_cat__________test</t>
-  </si>
-  <si>
-    <t>weekly_dog__________test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -348,12 +358,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -670,25 +679,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E1" sqref="E1:K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" customWidth="1"/>
+    <col min="1" max="1" width="23.625" customWidth="1"/>
+    <col min="3" max="3" width="22.125" customWidth="1"/>
     <col min="4" max="4" width="25.5" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" customWidth="1"/>
+    <col min="6" max="6" width="23.375" customWidth="1"/>
     <col min="7" max="7" width="18.5" customWidth="1"/>
     <col min="8" max="8" width="37" customWidth="1"/>
-    <col min="9" max="9" width="20.33203125" customWidth="1"/>
+    <col min="9" max="9" width="20.375" customWidth="1"/>
     <col min="10" max="10" width="24.5" customWidth="1"/>
     <col min="11" max="11" width="32.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="17.100000000000001">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -723,7 +732,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -758,7 +767,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -793,7 +802,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -824,12 +833,12 @@
       <c r="J4" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:11" ht="17.100000000000001">
+      <c r="A5" t="s">
         <v>24</v>
       </c>
       <c r="B5" t="s">
@@ -857,8 +866,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:11" ht="17.100000000000001">
+      <c r="A6" t="s">
         <v>33</v>
       </c>
       <c r="B6" t="s">
@@ -886,8 +895,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:11" ht="17.100000000000001">
+      <c r="A7" t="s">
         <v>41</v>
       </c>
       <c r="B7" t="s">
@@ -921,20 +930,20 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="4" max="4" width="32.83203125" customWidth="1"/>
+    <col min="4" max="4" width="32.875" customWidth="1"/>
     <col min="5" max="5" width="34.5" customWidth="1"/>
-    <col min="6" max="6" width="35.1640625" customWidth="1"/>
+    <col min="6" max="6" width="35.125" customWidth="1"/>
     <col min="7" max="7" width="28.5" customWidth="1"/>
-    <col min="8" max="8" width="29.83203125" customWidth="1"/>
-    <col min="9" max="9" width="25.33203125" customWidth="1"/>
-    <col min="10" max="10" width="25.1640625" customWidth="1"/>
-    <col min="11" max="11" width="25.83203125" customWidth="1"/>
+    <col min="8" max="8" width="29.875" customWidth="1"/>
+    <col min="9" max="9" width="25.375" customWidth="1"/>
+    <col min="10" max="10" width="25.125" customWidth="1"/>
+    <col min="11" max="11" width="25.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="17.100000000000001">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -948,28 +957,28 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="F1" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="G1" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="H1" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="I1" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="J1" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1004,7 +1013,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1039,7 +1048,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1053,103 +1062,103 @@
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="G4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="I4" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="J4" t="s">
-        <v>60</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>76</v>
+        <v>55</v>
+      </c>
+      <c r="K4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="33.950000000000003">
+      <c r="A5" t="s">
+        <v>58</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D5" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="H5" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="J5" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="K5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>77</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="33.950000000000003">
+      <c r="A6" t="s">
+        <v>66</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6" t="s">
+        <v>71</v>
+      </c>
+      <c r="I6" t="s">
         <v>72</v>
       </c>
-      <c r="D6" t="s">
+      <c r="K6" t="s">
         <v>73</v>
       </c>
-      <c r="E6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" t="s">
-        <v>50</v>
-      </c>
-      <c r="H6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I6" t="s">
-        <v>52</v>
-      </c>
-      <c r="K6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>78</v>
+    </row>
+    <row r="7" spans="1:11" ht="33.950000000000003">
+      <c r="A7" t="s">
+        <v>74</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G7" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="K7" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>